<commit_message>
Added all current Data
</commit_message>
<xml_diff>
--- a/CompCars_Original/ResNet/Data_Full_EigenCAM_ResNet_CompCars_Original_ocrnet_hr48_carparts_noflip_23_08_2022.xlsx
+++ b/CompCars_Original/ResNet/Data_Full_EigenCAM_ResNet_CompCars_Original_ocrnet_hr48_carparts_noflip_23_08_2022.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,287 +436,349 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>segments</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>RawActivations</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>PercActivations</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>totalActivation</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>background</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>1827.09205168587</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>0.1451797787554805</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>168030528</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>back_bumper</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>83.98043758985914</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>0.006677752177250749</v>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>back_glass</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>77.98343752202911</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>0.006198398571733138</v>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>back_left_door</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>66.00469070271726</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>0.005239299980012199</v>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>back_left_light</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>73.17902572323301</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>0.005805456531627178</v>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>back_right_door</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>87.76321863641282</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>0.006956480043307339</v>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>back_right_light</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>97.74063914770061</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>0.00775480604796429</v>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>front_bumper</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>5515.390686685375</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>0.4377916207300939</v>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>front_glass</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>346.0842693736895</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>0.02768439132219819</v>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>front_left_door</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>40.18685983231494</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>0.003189413389586296</v>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>front_left_light</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="C12" t="n">
         <v>455.9929121867734</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>0.03610364052764825</v>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>front_right_door</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>34.36355093567691</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>0.002731846440683609</v>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>front_right_light</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="n">
         <v>262.6156498871453</v>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>0.02068338069428565</v>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>hood</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="C15" t="n">
         <v>3526.999225092294</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>0.2794868421682471</v>
       </c>
-      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>left_mirror</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="C16" t="n">
         <v>6.586750167062902</v>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>0.0005218749087548442</v>
       </c>
-      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>right_mirror</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="C17" t="n">
         <v>2.196912456393991</v>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>0.0001723338791835631</v>
       </c>
-      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>tailgate</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="C18" t="n">
         <v>4.534295576591363</v>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>0.000360356445869738</v>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>trunk</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="C19" t="n">
         <v>93.86987846415281</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>0.007458939931428028</v>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>wheel</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="C20" t="n">
         <v>0.04061890018903853</v>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>3.387300063320555e-06</v>
       </c>
-      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>